<commit_message>
ya sirve todo, falta sacar la funcion objetivo
</commit_message>
<xml_diff>
--- a/red/matriz_datos_resultados.xlsx
+++ b/red/matriz_datos_resultados.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\InterfazVisual_CalculoKIA\red\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PcR\Documents\GitHub\InterfazVisual_CalculoKIA_red\red\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DBB3EE-4D7A-4010-9E52-55C7D926A0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9252" activeTab="1"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Limpio" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -101,7 +102,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,7 +342,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -665,24 +666,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" activeCellId="6" sqref="A1:A1048576 B1:B1048576 C1:C1048576 D1:D1048576 E1:E1048576 F1:F1048576 J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="8" width="8.77734375" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -720,7 +721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.125</v>
       </c>
@@ -752,7 +753,7 @@
         <v>8.7301036313086567E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.125</v>
       </c>
@@ -784,7 +785,7 @@
         <v>8.7384065439818882E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.125</v>
       </c>
@@ -816,7 +817,7 @@
         <v>8.744759934187342E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.125</v>
       </c>
@@ -848,7 +849,7 @@
         <v>8.7721765782072672E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.125</v>
       </c>
@@ -880,7 +881,7 @@
         <v>8.7632532638294352E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.125</v>
       </c>
@@ -924,7 +925,7 @@
       <c r="U7" s="18"/>
       <c r="V7" s="19"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.125</v>
       </c>
@@ -978,7 +979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.125</v>
       </c>
@@ -1040,7 +1041,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.125</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>8.1599999999999992E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.125</v>
       </c>
@@ -1137,7 +1138,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.125</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.125</v>
       </c>
@@ -1204,7 +1205,7 @@
         <v>1.1066917874793111E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.125</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>1.103807449598936E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.125</v>
       </c>
@@ -1268,7 +1269,7 @@
         <v>1.1027023804855379E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.125</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>1.102744983007627E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.125</v>
       </c>
@@ -1332,7 +1333,7 @@
         <v>1.1061700306261161E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.125</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>1.103999456925061E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.125</v>
       </c>
@@ -1396,7 +1397,7 @@
         <v>1.1095825964791009E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.125</v>
       </c>
@@ -1428,7 +1429,7 @@
         <v>1.103807449598936E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.125</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>1.1062342234087661E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.125</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>1.2553450571071119E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.125</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>1.288416173365219E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.125</v>
       </c>
@@ -1556,7 +1557,7 @@
         <v>1.3218465666053969E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.125</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>1.3730115618762399E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.125</v>
       </c>
@@ -1620,7 +1621,7 @@
         <v>1.373891156067832E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.125</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>1.3392189531162509E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.125</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>1.275166592865574E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.125</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>1.318466461295268E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.125</v>
       </c>
@@ -1748,7 +1749,7 @@
         <v>1.2849939390371071E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.125</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>2.27801248866715E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.125</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>2.2777878022977498E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.125</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>2.2788474565523589E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.125</v>
       </c>
@@ -1876,7 +1877,7 @@
         <v>2.2773122232570631E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.125</v>
       </c>
@@ -1908,7 +1909,7 @@
         <v>2.2784331157952981E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.125</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>2.277944922774818E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.125</v>
       </c>
@@ -1972,7 +1973,7 @@
         <v>2.2779893514088241E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.125</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>2.2788474565523589E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.125</v>
       </c>
@@ -2036,7 +2037,7 @@
         <v>2.2786755877729809E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.125</v>
       </c>
@@ -2068,7 +2069,7 @@
         <v>2.279043409767062E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.125</v>
       </c>
@@ -2100,7 +2101,7 @@
         <v>3.5975643317937771E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.125</v>
       </c>
@@ -2132,7 +2133,7 @@
         <v>3.434003881497213E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.125</v>
       </c>
@@ -2164,7 +2165,7 @@
         <v>3.3560073598156571E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.125</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>3.3714236162746981E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.125</v>
       </c>
@@ -2228,7 +2229,7 @@
         <v>3.3605156809011221E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.125</v>
       </c>
@@ -2260,7 +2261,7 @@
         <v>3.297495457895103E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.125</v>
       </c>
@@ -2292,7 +2293,7 @@
         <v>3.3342633025510082E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.125</v>
       </c>
@@ -2324,7 +2325,7 @@
         <v>3.347354302234378E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.125</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>3.34080002843146E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.125</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>3.325518762927711E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2420,7 +2421,7 @@
         <v>3.7461629205079618E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>3.8101484521639389E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2484,7 +2485,7 @@
         <v>3.7461629205079618E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2516,7 +2517,7 @@
         <v>3.7705994484446022E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2548,7 +2549,7 @@
         <v>3.7705994484446022E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2580,7 +2581,7 @@
         <v>3.7705994484446022E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2612,7 +2613,7 @@
         <v>3.75836333155685E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2644,7 +2645,7 @@
         <v>3.75836333155685E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2676,7 +2677,7 @@
         <v>3.75836333155685E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2708,7 +2709,7 @@
         <v>3.7461629205079618E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>6.2532954554992836E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2772,7 +2773,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2836,7 +2837,7 @@
         <v>6.294858673920481E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2868,7 +2869,7 @@
         <v>6.250241975719491E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2932,7 +2933,7 @@
         <v>6.1875542252874346E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -2996,7 +2997,7 @@
         <v>6.2073295229088539E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3028,7 +3029,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3060,7 +3061,7 @@
         <v>7.3364237598696775E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3092,7 +3093,7 @@
         <v>7.2929784894196984E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3124,7 +3125,7 @@
         <v>7.3187343753959339E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3156,7 +3157,7 @@
         <v>7.2725993252441008E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>7.3187343753959339E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3220,7 +3221,7 @@
         <v>7.2725993252441008E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>7.2929784894196984E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3284,7 +3285,7 @@
         <v>7.3187343753959339E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3316,7 +3317,7 @@
         <v>7.3364237598696775E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3348,7 +3349,7 @@
         <v>7.3581993485846578E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3380,7 +3381,7 @@
         <v>1.2328182127672501E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>1.21642491713172E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3444,7 +3445,7 @@
         <v>1.1980637361870201E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3476,7 +3477,7 @@
         <v>1.200368558641635E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3508,7 +3509,7 @@
         <v>1.21642491713172E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3540,7 +3541,7 @@
         <v>1.200368558641635E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3572,7 +3573,7 @@
         <v>1.182384112120917E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3604,7 +3605,7 @@
         <v>1.2328182127672501E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3636,7 +3637,7 @@
         <v>1.1980637361870201E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3668,7 +3669,7 @@
         <v>1.200368558641635E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3700,7 +3701,7 @@
         <v>3.330153910257629E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3732,7 +3733,7 @@
         <v>3.411441822074908E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3764,7 +3765,7 @@
         <v>3.411441822074908E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3796,7 +3797,7 @@
         <v>3.1847613352400752E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3828,7 +3829,7 @@
         <v>3.330153910257629E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3860,7 +3861,7 @@
         <v>3.330153910257629E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>3.1956939747968031E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3924,7 +3925,7 @@
         <v>3.330153910257629E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3956,7 +3957,7 @@
         <v>3.1956939747968031E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -3988,7 +3989,7 @@
         <v>3.411441822074908E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0.12280000000000001</v>
       </c>
@@ -4020,7 +4021,7 @@
         <v>9.8470440023758427E-4</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0.12280000000000001</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>9.7804461034213508E-4</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0.12280000000000001</v>
       </c>
@@ -4084,7 +4085,7 @@
         <v>9.8128121566502823E-4</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0.12280000000000001</v>
       </c>
@@ -4116,7 +4117,7 @@
         <v>9.7464120897591496E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0.12280000000000001</v>
       </c>
@@ -4148,7 +4149,7 @@
         <v>9.7804461034213508E-4</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0.12280000000000001</v>
       </c>
@@ -4180,7 +4181,7 @@
         <v>9.7464120897591496E-4</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0.12280000000000001</v>
       </c>
@@ -4212,7 +4213,7 @@
         <v>9.8470440023758427E-4</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0.12280000000000001</v>
       </c>
@@ -4244,7 +4245,7 @@
         <v>9.8128121566502823E-4</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0.12280000000000001</v>
       </c>
@@ -4276,7 +4277,7 @@
         <v>9.7827409054165241E-4</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0.12280000000000001</v>
       </c>
@@ -4308,7 +4309,7 @@
         <v>9.8470440023758427E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0.12280000000000001</v>
       </c>
@@ -4340,7 +4341,7 @@
         <v>1.642122872615835E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0.12280000000000001</v>
       </c>
@@ -4372,7 +4373,7 @@
         <v>1.654486012840223E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0.12280000000000001</v>
       </c>
@@ -4404,7 +4405,7 @@
         <v>1.6482946714493399E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0.12280000000000001</v>
       </c>
@@ -4436,7 +4437,7 @@
         <v>1.660316790772652E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0.12280000000000001</v>
       </c>
@@ -4468,7 +4469,7 @@
         <v>1.6482946714493399E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0.12280000000000001</v>
       </c>
@@ -4500,7 +4501,7 @@
         <v>1.6482946714493399E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0.12280000000000001</v>
       </c>
@@ -4532,7 +4533,7 @@
         <v>1.660316790772652E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0.12280000000000001</v>
       </c>
@@ -4564,7 +4565,7 @@
         <v>1.6537131157616459E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0.12280000000000001</v>
       </c>
@@ -4596,7 +4597,7 @@
         <v>1.654486012840223E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0.12280000000000001</v>
       </c>
@@ -4628,7 +4629,7 @@
         <v>1.6537131157616459E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0.12280000000000001</v>
       </c>
@@ -4660,7 +4661,7 @@
         <v>2.5975431068038781E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0.12280000000000001</v>
       </c>
@@ -4692,7 +4693,7 @@
         <v>2.5963864976567708E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0.12280000000000001</v>
       </c>
@@ -4724,7 +4725,7 @@
         <v>2.6133842288758569E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0.12280000000000001</v>
       </c>
@@ -4756,7 +4757,7 @@
         <v>2.5963864976567708E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0.12280000000000001</v>
       </c>
@@ -4788,7 +4789,7 @@
         <v>2.5963864976567708E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0.12280000000000001</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>2.6133842288758569E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0.12280000000000001</v>
       </c>
@@ -4852,7 +4853,7 @@
         <v>2.6056119882288098E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0.12280000000000001</v>
       </c>
@@ -4884,7 +4885,7 @@
         <v>2.6228524390766732E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0.12280000000000001</v>
       </c>
@@ -4916,7 +4917,7 @@
         <v>2.5963864976567708E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>0.12280000000000001</v>
       </c>
@@ -4948,7 +4949,7 @@
         <v>9.914707090329284E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0.12280000000000001</v>
       </c>
@@ -4980,7 +4981,7 @@
         <v>9.6737880592825919E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>0.12280000000000001</v>
       </c>
@@ -5012,7 +5013,7 @@
         <v>9.1761115841781961E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>0.12280000000000001</v>
       </c>
@@ -5044,7 +5045,7 @@
         <v>9.914707090329284E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>0.12280000000000001</v>
       </c>
@@ -5076,7 +5077,7 @@
         <v>1.0472585847982E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>0.12280000000000001</v>
       </c>
@@ -5108,7 +5109,7 @@
         <v>9.1761115841781961E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>0.12280000000000001</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>9.4393800575394166E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>0.12280000000000001</v>
       </c>
@@ -5172,7 +5173,7 @@
         <v>9.6737880592825919E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>0.12280000000000001</v>
       </c>
@@ -5204,7 +5205,7 @@
         <v>9.4393800575394166E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>0.12280000000000001</v>
       </c>
@@ -5245,19 +5246,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5280,7 +5281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.125</v>
       </c>
@@ -5303,7 +5304,7 @@
         <v>8.7301036313086567E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.125</v>
       </c>
@@ -5326,7 +5327,7 @@
         <v>8.7384065439818882E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.125</v>
       </c>
@@ -5349,7 +5350,7 @@
         <v>8.744759934187342E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.125</v>
       </c>
@@ -5372,7 +5373,7 @@
         <v>8.7721765782072672E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.125</v>
       </c>
@@ -5395,7 +5396,7 @@
         <v>8.7632532638294352E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.125</v>
       </c>
@@ -5418,7 +5419,7 @@
         <v>8.7636459530776784E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.125</v>
       </c>
@@ -5441,7 +5442,7 @@
         <v>8.7648242320118995E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.125</v>
       </c>
@@ -5464,7 +5465,7 @@
         <v>8.7717832952403008E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.125</v>
       </c>
@@ -5487,7 +5488,7 @@
         <v>8.7572816563263E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.125</v>
       </c>
@@ -5510,7 +5511,7 @@
         <v>8.7368423084008577E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.125</v>
       </c>
@@ -5533,7 +5534,7 @@
         <v>1.1074923077653009E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.125</v>
       </c>
@@ -5556,7 +5557,7 @@
         <v>1.1066917874793111E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.125</v>
       </c>
@@ -5579,7 +5580,7 @@
         <v>1.103807449598936E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.125</v>
       </c>
@@ -5602,7 +5603,7 @@
         <v>1.1027023804855379E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.125</v>
       </c>
@@ -5625,7 +5626,7 @@
         <v>1.102744983007627E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.125</v>
       </c>
@@ -5648,7 +5649,7 @@
         <v>1.1061700306261161E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.125</v>
       </c>
@@ -5671,7 +5672,7 @@
         <v>1.103999456925061E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.125</v>
       </c>
@@ -5694,7 +5695,7 @@
         <v>1.1095825964791009E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.125</v>
       </c>
@@ -5717,7 +5718,7 @@
         <v>1.103807449598936E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.125</v>
       </c>
@@ -5740,7 +5741,7 @@
         <v>1.1062342234087661E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.125</v>
       </c>
@@ -5763,7 +5764,7 @@
         <v>1.2553450571071119E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.125</v>
       </c>
@@ -5786,7 +5787,7 @@
         <v>1.288416173365219E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.125</v>
       </c>
@@ -5809,7 +5810,7 @@
         <v>1.3218465666053969E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.125</v>
       </c>
@@ -5832,7 +5833,7 @@
         <v>1.3730115618762399E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.125</v>
       </c>
@@ -5855,7 +5856,7 @@
         <v>1.373891156067832E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.125</v>
       </c>
@@ -5878,7 +5879,7 @@
         <v>1.3392189531162509E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.125</v>
       </c>
@@ -5901,7 +5902,7 @@
         <v>1.275166592865574E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.125</v>
       </c>
@@ -5924,7 +5925,7 @@
         <v>1.318466461295268E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.125</v>
       </c>
@@ -5947,7 +5948,7 @@
         <v>1.2849939390371071E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.125</v>
       </c>
@@ -5970,7 +5971,7 @@
         <v>2.27801248866715E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.125</v>
       </c>
@@ -5993,7 +5994,7 @@
         <v>2.2777878022977498E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.125</v>
       </c>
@@ -6016,7 +6017,7 @@
         <v>2.2788474565523589E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.125</v>
       </c>
@@ -6039,7 +6040,7 @@
         <v>2.2773122232570631E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.125</v>
       </c>
@@ -6062,7 +6063,7 @@
         <v>2.2784331157952981E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.125</v>
       </c>
@@ -6085,7 +6086,7 @@
         <v>2.277944922774818E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.125</v>
       </c>
@@ -6108,7 +6109,7 @@
         <v>2.2779893514088241E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.125</v>
       </c>
@@ -6131,7 +6132,7 @@
         <v>2.2788474565523589E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.125</v>
       </c>
@@ -6154,7 +6155,7 @@
         <v>2.2786755877729809E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.125</v>
       </c>
@@ -6177,7 +6178,7 @@
         <v>2.279043409767062E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.125</v>
       </c>
@@ -6200,7 +6201,7 @@
         <v>3.5975643317937771E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.125</v>
       </c>
@@ -6223,7 +6224,7 @@
         <v>3.434003881497213E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.125</v>
       </c>
@@ -6246,7 +6247,7 @@
         <v>3.3560073598156571E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.125</v>
       </c>
@@ -6269,7 +6270,7 @@
         <v>3.3714236162746981E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.125</v>
       </c>
@@ -6292,7 +6293,7 @@
         <v>3.3605156809011221E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.125</v>
       </c>
@@ -6315,7 +6316,7 @@
         <v>3.297495457895103E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.125</v>
       </c>
@@ -6338,7 +6339,7 @@
         <v>3.3342633025510082E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.125</v>
       </c>
@@ -6361,7 +6362,7 @@
         <v>3.347354302234378E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.125</v>
       </c>
@@ -6384,7 +6385,7 @@
         <v>3.34080002843146E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.125</v>
       </c>
@@ -6407,7 +6408,7 @@
         <v>3.325518762927711E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6430,7 +6431,7 @@
         <v>3.7461629205079618E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6453,7 +6454,7 @@
         <v>3.8101484521639389E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6476,7 +6477,7 @@
         <v>3.7461629205079618E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6499,7 +6500,7 @@
         <v>3.7705994484446022E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6522,7 +6523,7 @@
         <v>3.7705994484446022E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6545,7 +6546,7 @@
         <v>3.7705994484446022E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6568,7 +6569,7 @@
         <v>3.75836333155685E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6591,7 +6592,7 @@
         <v>3.75836333155685E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6614,7 +6615,7 @@
         <v>3.75836333155685E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6637,7 +6638,7 @@
         <v>3.7461629205079618E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6660,7 +6661,7 @@
         <v>6.2532954554992836E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6683,7 +6684,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6706,7 +6707,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6729,7 +6730,7 @@
         <v>6.294858673920481E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6752,7 +6753,7 @@
         <v>6.250241975719491E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6775,7 +6776,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6798,7 +6799,7 @@
         <v>6.1875542252874346E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6821,7 +6822,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6844,7 +6845,7 @@
         <v>6.2073295229088539E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6867,7 +6868,7 @@
         <v>6.2287563359644338E-4</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6890,7 +6891,7 @@
         <v>7.3364237598696775E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6913,7 +6914,7 @@
         <v>7.2929784894196984E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6936,7 +6937,7 @@
         <v>7.3187343753959339E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6959,7 +6960,7 @@
         <v>7.2725993252441008E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -6982,7 +6983,7 @@
         <v>7.3187343753959339E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7005,7 +7006,7 @@
         <v>7.2725993252441008E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7028,7 +7029,7 @@
         <v>7.2929784894196984E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7051,7 +7052,7 @@
         <v>7.3187343753959339E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7074,7 +7075,7 @@
         <v>7.3364237598696775E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7097,7 +7098,7 @@
         <v>7.3581993485846578E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7120,7 +7121,7 @@
         <v>1.2328182127672501E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7143,7 +7144,7 @@
         <v>1.21642491713172E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7166,7 +7167,7 @@
         <v>1.1980637361870201E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7189,7 +7190,7 @@
         <v>1.200368558641635E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7212,7 +7213,7 @@
         <v>1.21642491713172E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7235,7 +7236,7 @@
         <v>1.200368558641635E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7258,7 +7259,7 @@
         <v>1.182384112120917E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7281,7 +7282,7 @@
         <v>1.2328182127672501E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7304,7 +7305,7 @@
         <v>1.1980637361870201E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7327,7 +7328,7 @@
         <v>1.200368558641635E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7350,7 +7351,7 @@
         <v>3.330153910257629E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7373,7 +7374,7 @@
         <v>3.411441822074908E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7396,7 +7397,7 @@
         <v>3.411441822074908E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7419,7 +7420,7 @@
         <v>3.1847613352400752E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7442,7 +7443,7 @@
         <v>3.330153910257629E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>3.330153910257629E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7488,7 +7489,7 @@
         <v>3.1956939747968031E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7511,7 +7512,7 @@
         <v>3.330153910257629E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7534,7 +7535,7 @@
         <v>3.1956939747968031E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5.1700000000000003E-2</v>
       </c>
@@ -7557,7 +7558,7 @@
         <v>3.411441822074908E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0.12280000000000001</v>
       </c>
@@ -7580,7 +7581,7 @@
         <v>9.8470440023758427E-4</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0.12280000000000001</v>
       </c>
@@ -7603,7 +7604,7 @@
         <v>9.7804461034213508E-4</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0.12280000000000001</v>
       </c>
@@ -7626,7 +7627,7 @@
         <v>9.8128121566502823E-4</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0.12280000000000001</v>
       </c>
@@ -7649,7 +7650,7 @@
         <v>9.7464120897591496E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0.12280000000000001</v>
       </c>
@@ -7672,7 +7673,7 @@
         <v>9.7804461034213508E-4</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0.12280000000000001</v>
       </c>
@@ -7695,7 +7696,7 @@
         <v>9.7464120897591496E-4</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0.12280000000000001</v>
       </c>
@@ -7718,7 +7719,7 @@
         <v>9.8470440023758427E-4</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0.12280000000000001</v>
       </c>
@@ -7741,7 +7742,7 @@
         <v>9.8128121566502823E-4</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0.12280000000000001</v>
       </c>
@@ -7764,7 +7765,7 @@
         <v>9.7827409054165241E-4</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0.12280000000000001</v>
       </c>
@@ -7787,7 +7788,7 @@
         <v>9.8470440023758427E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0.12280000000000001</v>
       </c>
@@ -7810,7 +7811,7 @@
         <v>1.642122872615835E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0.12280000000000001</v>
       </c>
@@ -7833,7 +7834,7 @@
         <v>1.654486012840223E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0.12280000000000001</v>
       </c>
@@ -7856,7 +7857,7 @@
         <v>1.6482946714493399E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0.12280000000000001</v>
       </c>
@@ -7879,7 +7880,7 @@
         <v>1.660316790772652E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0.12280000000000001</v>
       </c>
@@ -7902,7 +7903,7 @@
         <v>1.6482946714493399E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0.12280000000000001</v>
       </c>
@@ -7925,7 +7926,7 @@
         <v>1.6482946714493399E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0.12280000000000001</v>
       </c>
@@ -7948,7 +7949,7 @@
         <v>1.660316790772652E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0.12280000000000001</v>
       </c>
@@ -7971,7 +7972,7 @@
         <v>1.6537131157616459E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0.12280000000000001</v>
       </c>
@@ -7994,7 +7995,7 @@
         <v>1.654486012840223E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0.12280000000000001</v>
       </c>
@@ -8017,7 +8018,7 @@
         <v>1.6537131157616459E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0.12280000000000001</v>
       </c>
@@ -8040,7 +8041,7 @@
         <v>2.5975431068038781E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0.12280000000000001</v>
       </c>
@@ -8063,7 +8064,7 @@
         <v>2.5963864976567708E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0.12280000000000001</v>
       </c>
@@ -8086,7 +8087,7 @@
         <v>2.6133842288758569E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0.12280000000000001</v>
       </c>
@@ -8109,7 +8110,7 @@
         <v>2.5963864976567708E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0.12280000000000001</v>
       </c>
@@ -8132,7 +8133,7 @@
         <v>2.5963864976567708E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0.12280000000000001</v>
       </c>
@@ -8155,7 +8156,7 @@
         <v>2.6133842288758569E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0.12280000000000001</v>
       </c>
@@ -8178,7 +8179,7 @@
         <v>2.6056119882288098E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0.12280000000000001</v>
       </c>
@@ -8201,7 +8202,7 @@
         <v>2.6228524390766732E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0.12280000000000001</v>
       </c>
@@ -8224,7 +8225,7 @@
         <v>2.5963864976567708E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>0.12280000000000001</v>
       </c>
@@ -8247,7 +8248,7 @@
         <v>9.914707090329284E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0.12280000000000001</v>
       </c>
@@ -8270,7 +8271,7 @@
         <v>9.6737880592825919E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>0.12280000000000001</v>
       </c>
@@ -8293,7 +8294,7 @@
         <v>9.1761115841781961E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>0.12280000000000001</v>
       </c>
@@ -8316,7 +8317,7 @@
         <v>9.914707090329284E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>0.12280000000000001</v>
       </c>
@@ -8339,7 +8340,7 @@
         <v>1.0472585847982E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>0.12280000000000001</v>
       </c>
@@ -8362,7 +8363,7 @@
         <v>9.1761115841781961E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>0.12280000000000001</v>
       </c>
@@ -8385,7 +8386,7 @@
         <v>9.4393800575394166E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>0.12280000000000001</v>
       </c>
@@ -8408,7 +8409,7 @@
         <v>9.6737880592825919E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>0.12280000000000001</v>
       </c>
@@ -8431,7 +8432,7 @@
         <v>9.4393800575394166E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>0.12280000000000001</v>
       </c>

</xml_diff>

<commit_message>
Quite todo lo de Shulman y Cornell, tambien puse todo en ingles. Falta cambiar lo de Morelos
</commit_message>
<xml_diff>
--- a/red/matriz_datos_resultados.xlsx
+++ b/red/matriz_datos_resultados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PcR\Documents\GitHub\InterfazVisual_CalculoKIA_red\red\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DBB3EE-4D7A-4010-9E52-55C7D926A0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C8FEAA-C786-46AC-9FD9-09CB29155D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5247,7 +5247,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
@@ -5258,7 +5258,7 @@
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.125</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>8.7301036313086567E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.125</v>
       </c>
@@ -5326,8 +5326,12 @@
       <c r="G3">
         <v>8.7384065439818882E-4</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f>_xlfn.STDEV.S(G2:G139)</f>
+        <v>2.2949620245395702E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.125</v>
       </c>
@@ -5350,7 +5354,7 @@
         <v>8.744759934187342E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.125</v>
       </c>
@@ -5373,7 +5377,7 @@
         <v>8.7721765782072672E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.125</v>
       </c>
@@ -5396,7 +5400,7 @@
         <v>8.7632532638294352E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.125</v>
       </c>
@@ -5419,7 +5423,7 @@
         <v>8.7636459530776784E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.125</v>
       </c>
@@ -5442,7 +5446,7 @@
         <v>8.7648242320118995E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.125</v>
       </c>
@@ -5465,7 +5469,7 @@
         <v>8.7717832952403008E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.125</v>
       </c>
@@ -5488,7 +5492,7 @@
         <v>8.7572816563263E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.125</v>
       </c>
@@ -5511,7 +5515,7 @@
         <v>8.7368423084008577E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.125</v>
       </c>
@@ -5534,7 +5538,7 @@
         <v>1.1074923077653009E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.125</v>
       </c>
@@ -5557,7 +5561,7 @@
         <v>1.1066917874793111E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.125</v>
       </c>
@@ -5580,7 +5584,7 @@
         <v>1.103807449598936E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.125</v>
       </c>
@@ -5603,7 +5607,7 @@
         <v>1.1027023804855379E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.125</v>
       </c>

</xml_diff>